<commit_message>
GAP-10 added scrip to upload rasters in geoserver and  updated requirements
</commit_message>
<xml_diff>
--- a/src/database.xlsx
+++ b/src/database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LGA\Scripts\spcat_scripts\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\spcat_scripts\spcat_scripts\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF4BA4F-8455-4F34-B705-6C3B40535114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A59E05-A9FC-43AF-BF0C-E891CF71EDC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,10 +43,10 @@
     <t>name_db</t>
   </si>
   <si>
+    <t>port</t>
+  </si>
+  <si>
     <t>dbgap</t>
-  </si>
-  <si>
-    <t>port</t>
   </si>
 </sst>
 </file>
@@ -411,16 +411,16 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,17 +428,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -446,17 +446,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>8</v>
       </c>
       <c r="B6" s="2">
         <v>27017</v>

</xml_diff>

<commit_message>
GAP-10 added geoserver data to config file
</commit_message>
<xml_diff>
--- a/src/database.xlsx
+++ b/src/database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\spcat_scripts\spcat_scripts\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A59E05-A9FC-43AF-BF0C-E891CF71EDC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5956C2-87F3-44B3-A065-D818013EABFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>parameter</t>
   </si>
@@ -46,14 +46,29 @@
     <t>port</t>
   </si>
   <si>
-    <t>dbgap</t>
+    <t>user_gs</t>
+  </si>
+  <si>
+    <t>pass_gs</t>
+  </si>
+  <si>
+    <t>workspace_gs</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>geo_url</t>
+  </si>
+  <si>
+    <t>db_gap</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,6 +81,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -92,10 +115,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -103,8 +127,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -408,10 +434,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -451,7 +477,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -462,7 +488,35 @@
         <v>27017</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added comands in pipeline
</commit_message>
<xml_diff>
--- a/src/database.xlsx
+++ b/src/database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\spcat_scripts\spcat_scripts\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5956C2-87F3-44B3-A065-D818013EABFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01F0807-F52F-4952-A673-C4E166A8225C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -119,7 +119,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -128,6 +128,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -437,7 +438,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -508,6 +509,7 @@
       <c r="A10" t="s">
         <v>11</v>
       </c>
+      <c r="B10" s="4"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">

</xml_diff>